<commit_message>
This commit include 1st coding test file
</commit_message>
<xml_diff>
--- a/Coding Test/Coding Test Excel 1.xlsx
+++ b/Coding Test/Coding Test Excel 1.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NIHARIKA PANDA\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5163BCC3-F549-4781-BC79-9DE3A7C56EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19140" windowHeight="6840" activeTab="1"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
-    <pivotCache cacheId="8" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>Product</t>
   </si>
@@ -91,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -268,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -289,9 +295,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -310,7 +313,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -324,12 +329,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Abhavya Singh" refreshedDate="45510.459675231483" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="10">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Abhavya Singh" refreshedDate="45510.459675231483" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="10" xr:uid="{00000000-000A-0000-FFFF-FFFF05000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:D11" sheet="Sheet1"/>
   </cacheSource>
@@ -366,7 +374,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Abhavya Singh" refreshedDate="45510.467789236114" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="10">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Abhavya Singh" refreshedDate="45510.467789236114" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="10" xr:uid="{00000000-000A-0000-FFFF-FFFF08000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="D1:G11" sheet="Sheet1"/>
   </cacheSource>
@@ -528,7 +536,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A13:C30" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="4">
     <pivotField numFmtId="14" showAll="0"/>
@@ -541,12 +549,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -614,14 +625,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -659,7 +673,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -731,7 +745,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -904,26 +918,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="4"/>
+    <col min="5" max="5" width="9.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.77734375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="4:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
@@ -937,7 +951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="4:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D2" s="6">
         <v>45292</v>
       </c>
@@ -951,7 +965,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="3" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="4:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D3" s="6">
         <v>45293</v>
       </c>
@@ -965,7 +979,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="4" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="4:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D4" s="6">
         <v>45294</v>
       </c>
@@ -979,7 +993,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="5" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="4:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D5" s="6">
         <v>45295</v>
       </c>
@@ -993,7 +1007,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="6" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="4:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D6" s="6">
         <v>45296</v>
       </c>
@@ -1007,7 +1021,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="7" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="4:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D7" s="6">
         <v>45297</v>
       </c>
@@ -1021,7 +1035,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="8" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="4:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="6">
         <v>45298</v>
       </c>
@@ -1035,7 +1049,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="4:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="6">
         <v>45299</v>
       </c>
@@ -1049,7 +1063,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="10" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="4:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="6">
         <v>45300</v>
       </c>
@@ -1063,7 +1077,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="11" spans="4:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="4:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="6">
         <v>45301</v>
       </c>
@@ -1084,208 +1098,199 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
       <c r="F1">
         <f>SUMIF(Sheet1!E1:E11,"Product A",Sheet1!G1:G11)</f>
         <v>3600</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
       <c r="F2">
-        <f>MAX(C6:C7)</f>
+        <f>AVERAGEIF(Sheet1!F1:F11,"South",Sheet1!G1:G11)</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3">
+        <f>_xlfn.MAXIFS(Sheet1!G1:G11,Sheet1!F1:F11,"West")</f>
         <v>850</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-    </row>
-    <row r="5" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22">
-        <v>1</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="22">
-        <f>VLOOKUP(B6,Sheet1!F1:G11,2,0)</f>
-        <v>700</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22">
-        <v>2</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="22">
-        <v>850</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="8" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-    </row>
-    <row r="9" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="14"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="14"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="14"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="14"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="14"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17"/>
+    <row r="4" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="14"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1298,123 +1303,123 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5">
         <v>1700</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6">
         <v>1700</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7">
         <v>3600</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8">
         <v>3600</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9">
         <v>4500</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10">
         <v>4500</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11">
         <v>1550</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12">
         <v>1550</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13">
         <v>11350</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="1:2" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="1:3" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1423,7 +1428,7 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>45292</v>
       </c>
@@ -1432,7 +1437,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>45293</v>
       </c>
@@ -1441,7 +1446,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>45294</v>
       </c>
@@ -1450,7 +1455,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>45295</v>
       </c>
@@ -1459,7 +1464,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>45296</v>
       </c>
@@ -1468,7 +1473,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>45297</v>
       </c>
@@ -1477,7 +1482,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>45298</v>
       </c>
@@ -1486,7 +1491,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>45299</v>
       </c>
@@ -1495,7 +1500,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>45300</v>
       </c>
@@ -1504,7 +1509,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>45301</v>
       </c>

</xml_diff>